<commit_message>
calculos, paros y scheule
</commit_message>
<xml_diff>
--- a/public/storage/Archivos/FormatosExcel/Carga_Masiva.xlsx
+++ b/public/storage/Archivos/FormatosExcel/Carga_Masiva.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinCR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB3C0A1-E2F4-468D-A4A5-587B331B7BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B91D24-0890-4D20-949E-B69510912D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71AC2B83-B0D1-4BB0-BA54-74FED2C5CE57}"/>
   </bookViews>
@@ -26,30 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>operador</t>
-  </si>
-  <si>
-    <t>clave</t>
-  </si>
-  <si>
-    <t>equipo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>fecha</t>
-  </si>
-  <si>
-    <t>partida</t>
   </si>
   <si>
     <t>peso</t>
   </si>
   <si>
-    <t>proceso</t>
+    <t>turno</t>
   </si>
   <si>
-    <t>maquina</t>
+    <t>paquete_operador</t>
+  </si>
+  <si>
+    <t>paquete_norma</t>
   </si>
 </sst>
 </file>
@@ -402,87 +393,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A784B74C-288C-4781-8FDB-9DE2BD6605E2}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>